<commit_message>
Add functionality to send all photos from a folder and update bot token
</commit_message>
<xml_diff>
--- a/user2.xlsx
+++ b/user2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>ᴍᴀᴛᴛ</t>
+  </si>
+  <si>
+    <t>Matin</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -453,6 +456,14 @@
         <v>1.03499497E8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>8.069824403E9</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1"/>

</xml_diff>